<commit_message>
improved dort by degree
</commit_message>
<xml_diff>
--- a/src/assets/data/Kidney_updated_R1_EMQverify6_21_2020.xlsx
+++ b/src/assets/data/Kidney_updated_R1_EMQverify6_21_2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hpaul/Work/CNS/ccf-asct-reporter/src/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hpaul/Work/CNS/ccf-asct-reporter/src/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F2BEC-A32E-034B-AB4C-B184E2CF06A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D789DB-E0AE-AE42-BA5D-482EDB6B9CED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="460" windowWidth="28040" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="460" windowWidth="35840" windowHeight="19760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kidney_updated_R1 copy" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>PDZK1IP1*, MT1G*</t>
   </si>
   <si>
-    <t>Loop of Henle, Thin Limb</t>
-  </si>
-  <si>
     <t>Descending Thin Limb Cell (general)</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
   </si>
   <si>
     <t>AQP1 low to none</t>
-  </si>
-  <si>
-    <t>Loop of Henle, Thick Limb</t>
   </si>
   <si>
     <t>Thick Ascending Limb Cell (general)</t>
@@ -641,6 +635,12 @@
   </si>
   <si>
     <t>renal artery[L/R]</t>
+  </si>
+  <si>
+    <t>Loop of Henle, Thin Limb</t>
+  </si>
+  <si>
+    <t>Loop of Henle, Thick Limb</t>
   </si>
 </sst>
 </file>
@@ -1496,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="K58" sqref="G58:K58"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="200" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1674,19 +1674,19 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1694,19 +1694,19 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>203</v>
       </c>
       <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
         <v>40</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>41</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1714,19 +1714,19 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>45</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1734,16 +1734,16 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1751,16 +1751,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1768,16 +1768,16 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>204</v>
       </c>
       <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
         <v>53</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1785,16 +1785,16 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" t="s">
         <v>56</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>57</v>
-      </c>
-      <c r="D16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1802,19 +1802,19 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1822,19 +1822,19 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
         <v>64</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -1842,19 +1842,19 @@
         <v>20</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="F19" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1862,16 +1862,16 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
         <v>73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1879,16 +1879,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
         <v>76</v>
-      </c>
-      <c r="D21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1896,16 +1896,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" t="s">
         <v>79</v>
-      </c>
-      <c r="D22" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1913,16 +1913,16 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" t="s">
         <v>82</v>
-      </c>
-      <c r="D23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="4" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -1930,19 +1930,19 @@
         <v>20</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="F24" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1950,16 +1950,16 @@
         <v>20</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" t="s">
         <v>90</v>
-      </c>
-      <c r="D25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1967,13 +1967,13 @@
         <v>20</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1981,13 +1981,13 @@
         <v>20</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1995,13 +1995,13 @@
         <v>20</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2009,16 +2009,16 @@
         <v>20</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
         <v>97</v>
-      </c>
-      <c r="D29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2026,16 +2026,16 @@
         <v>20</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" t="s">
         <v>100</v>
-      </c>
-      <c r="D30" t="s">
-        <v>101</v>
-      </c>
-      <c r="E30" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2043,16 +2043,16 @@
         <v>20</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C31" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>102</v>
+      </c>
+      <c r="E31" t="s">
         <v>103</v>
-      </c>
-      <c r="D31" t="s">
-        <v>104</v>
-      </c>
-      <c r="E31" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2060,16 +2060,16 @@
         <v>20</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" t="s">
         <v>106</v>
-      </c>
-      <c r="D32" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -2077,16 +2077,16 @@
         <v>20</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E33" t="s">
         <v>109</v>
-      </c>
-      <c r="D33" t="s">
-        <v>110</v>
-      </c>
-      <c r="E33" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2094,16 +2094,16 @@
         <v>20</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" t="s">
         <v>112</v>
-      </c>
-      <c r="D34" t="s">
-        <v>113</v>
-      </c>
-      <c r="E34" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2111,16 +2111,16 @@
         <v>20</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" t="s">
         <v>115</v>
-      </c>
-      <c r="D35" t="s">
-        <v>116</v>
-      </c>
-      <c r="E35" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2128,13 +2128,13 @@
         <v>20</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2142,406 +2142,406 @@
         <v>20</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D37" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" t="s">
         <v>122</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>123</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>124</v>
-      </c>
-      <c r="D38" t="s">
-        <v>125</v>
-      </c>
-      <c r="E38" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" t="s">
         <v>127</v>
       </c>
-      <c r="D39" t="s">
+      <c r="F39" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="E39" t="s">
-        <v>129</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B40" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C40" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" t="s">
         <v>131</v>
-      </c>
-      <c r="D40" t="s">
-        <v>132</v>
-      </c>
-      <c r="E40" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B41" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C41" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" t="s">
         <v>134</v>
-      </c>
-      <c r="D41" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B42" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" t="s">
         <v>137</v>
       </c>
-      <c r="D42" t="s">
+      <c r="F42" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="E42" t="s">
-        <v>139</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" t="s">
+        <v>140</v>
+      </c>
+      <c r="E43" t="s">
         <v>141</v>
-      </c>
-      <c r="D43" t="s">
-        <v>142</v>
-      </c>
-      <c r="E43" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>142</v>
+      </c>
+      <c r="B44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" t="s">
         <v>144</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
         <v>145</v>
       </c>
-      <c r="C44" t="s">
+      <c r="E44" t="s">
         <v>146</v>
-      </c>
-      <c r="D44" t="s">
-        <v>147</v>
-      </c>
-      <c r="E44" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B45" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C45" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" t="s">
         <v>149</v>
-      </c>
-      <c r="D45" t="s">
-        <v>150</v>
-      </c>
-      <c r="E45" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C46" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" t="s">
+        <v>151</v>
+      </c>
+      <c r="E46" t="s">
         <v>152</v>
-      </c>
-      <c r="D46" t="s">
-        <v>153</v>
-      </c>
-      <c r="E46" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B47" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" t="s">
         <v>155</v>
       </c>
-      <c r="C47" t="s">
+      <c r="E47" t="s">
         <v>156</v>
-      </c>
-      <c r="D47" t="s">
-        <v>157</v>
-      </c>
-      <c r="E47" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C48" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" t="s">
         <v>159</v>
-      </c>
-      <c r="D48" t="s">
-        <v>160</v>
-      </c>
-      <c r="E48" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B49" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C49" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" t="s">
+        <v>161</v>
+      </c>
+      <c r="E49" t="s">
         <v>162</v>
-      </c>
-      <c r="D49" t="s">
-        <v>163</v>
-      </c>
-      <c r="E49" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C50" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" t="s">
         <v>165</v>
-      </c>
-      <c r="D50" t="s">
-        <v>166</v>
-      </c>
-      <c r="E50" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C51" t="s">
+        <v>166</v>
+      </c>
+      <c r="D51" t="s">
+        <v>167</v>
+      </c>
+      <c r="E51" t="s">
         <v>168</v>
-      </c>
-      <c r="D51" t="s">
-        <v>169</v>
-      </c>
-      <c r="E51" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B52" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C52" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" t="s">
         <v>171</v>
-      </c>
-      <c r="D52" t="s">
-        <v>172</v>
-      </c>
-      <c r="E52" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C53" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" t="s">
+        <v>173</v>
+      </c>
+      <c r="E53" t="s">
         <v>174</v>
-      </c>
-      <c r="D53" t="s">
-        <v>175</v>
-      </c>
-      <c r="E53" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C54" t="s">
+        <v>175</v>
+      </c>
+      <c r="D54" t="s">
+        <v>176</v>
+      </c>
+      <c r="E54" t="s">
         <v>177</v>
-      </c>
-      <c r="D54" t="s">
-        <v>178</v>
-      </c>
-      <c r="E54" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B59" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F59" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G59" t="s">
+        <v>123</v>
+      </c>
+      <c r="H59" t="s">
         <v>124</v>
-      </c>
-      <c r="G59" t="s">
-        <v>125</v>
-      </c>
-      <c r="H59" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B60" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C60" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B61" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C61" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B62" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B63" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
+        <v>178</v>
+      </c>
+      <c r="B64" t="s">
+        <v>202</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B64" t="s">
-        <v>204</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="F64" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G64" t="s">
+        <v>126</v>
+      </c>
+      <c r="H64" t="s">
         <v>127</v>
-      </c>
-      <c r="G64" t="s">
-        <v>128</v>
-      </c>
-      <c r="H64" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B65" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>14</v>
@@ -2555,189 +2555,189 @@
     </row>
     <row r="66" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B66" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F66" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G66" t="s">
+        <v>126</v>
+      </c>
+      <c r="H66" t="s">
         <v>127</v>
-      </c>
-      <c r="G66" t="s">
-        <v>128</v>
-      </c>
-      <c r="H66" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D67" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F67" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G67" t="s">
+        <v>130</v>
+      </c>
+      <c r="H67" t="s">
         <v>131</v>
-      </c>
-      <c r="G67" t="s">
-        <v>132</v>
-      </c>
-      <c r="H67" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D68" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F68" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G68" t="s">
+        <v>133</v>
+      </c>
+      <c r="H68" t="s">
         <v>134</v>
-      </c>
-      <c r="G68" t="s">
-        <v>135</v>
-      </c>
-      <c r="H68" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B69" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D69" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G69" t="s">
+        <v>136</v>
+      </c>
+      <c r="H69" t="s">
         <v>137</v>
       </c>
-      <c r="G69" t="s">
+      <c r="I69" t="s">
         <v>138</v>
-      </c>
-      <c r="H69" t="s">
-        <v>139</v>
-      </c>
-      <c r="I69" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B70" t="s">
+        <v>186</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="F70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G70" t="s">
+        <v>123</v>
+      </c>
+      <c r="H70" t="s">
         <v>124</v>
-      </c>
-      <c r="G70" t="s">
-        <v>125</v>
-      </c>
-      <c r="H70" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B72" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C72" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B73" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C73" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B75" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F75" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G75" t="s">
+        <v>140</v>
+      </c>
+      <c r="H75" t="s">
         <v>141</v>
-      </c>
-      <c r="G75" t="s">
-        <v>142</v>
-      </c>
-      <c r="H75" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>191</v>
+      </c>
+      <c r="B76" t="s">
+        <v>192</v>
+      </c>
+      <c r="C76" t="s">
         <v>193</v>
-      </c>
-      <c r="B76" t="s">
-        <v>194</v>
-      </c>
-      <c r="C76" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B77" t="s">
+        <v>192</v>
+      </c>
+      <c r="C77" t="s">
         <v>194</v>
-      </c>
-      <c r="C77" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B78" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>